<commit_message>
about to finish sprint 2
</commit_message>
<xml_diff>
--- a/server/Resources/Files/coachExcel.xlsx
+++ b/server/Resources/Files/coachExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\droru\OneDrive\שולחן העבודה\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\WebstormProjects\wu-shu-project\server\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893FA5B0-8A73-4989-A92F-AF339EEC4190}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A360864-B5D6-4C46-B871-BD22003CE54C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,30 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sportclub</t>
+  </si>
+  <si>
+    <t>מספר מועדון</t>
+  </si>
+  <si>
+    <t>שם מועדון</t>
+  </si>
+  <si>
+    <t>הפנתרים</t>
+  </si>
+  <si>
+    <t>טאולו בע"מ</t>
+  </si>
+  <si>
+    <t>הנמרים</t>
+  </si>
+  <si>
+    <t>סאנדא רחובות</t>
+  </si>
+  <si>
+    <t>לוחמים בע"מ</t>
+  </si>
+  <si>
+    <t>הפועל בת ים</t>
+  </si>
+  <si>
+    <t>מיטב חדרה</t>
+  </si>
+  <si>
+    <t>קונגפו-פנדה</t>
+  </si>
+  <si>
     <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>sportclub</t>
   </si>
   <si>
     <t>teamname</t>
@@ -57,15 +87,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -73,15 +104,17 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,21 +138,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{926A92C3-48D0-48D9-86FC-370A287DE1C1}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -129,6 +191,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D11061F1-2CC4-4E4D-B1EC-017C7C2A643C}" name="טבלה1" displayName="טבלה1" ref="K2:L10" totalsRowShown="0">
+  <autoFilter ref="K2:L10" xr:uid="{9E9024D9-CE2C-4251-BF1F-6E220A974D4C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{469EAD23-0D3D-4A67-AAC2-B1881F08666B}" name="מספר מועדון"/>
+    <tableColumn id="2" xr3:uid="{989222B1-804C-4673-891F-E8BED60D0423}" name="שם מועדון"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,71 +467,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.69921875" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.296875" customWidth="1"/>
+    <col min="9" max="9" width="19.19921875" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.796875" customWidth="1"/>
+    <col min="12" max="12" width="16.3984375" customWidth="1"/>
+    <col min="14" max="14" width="13.3984375" customWidth="1"/>
+    <col min="15" max="15" width="14.59765625" customWidth="1"/>
+    <col min="16" max="16" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2"/>
-      <c r="F2" s="3"/>
       <c r="G2" s="2"/>
-      <c r="K2" s="4"/>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="תאריך לא תקין" error="נא הכנס תאריך בפורמט תקין_x000a_" promptTitle="תאריך לידה " prompt="נא הכנס תאריך בפורמט mm/dd/yyyy" sqref="G3:G1048576" xr:uid="{417E5E27-42F6-4189-8503-9F24241A0227}">
-      <formula1>1</formula1>
+  <dataValidations count="9">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="תאריך לידה " prompt="נא הכנס תאריך לידה בפורמט: _x000a_dd/mm/yyyy" sqref="F1:F1048576" xr:uid="{A983D1A3-FE83-4624-8258-6A8B9098F02C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="ת.ז" prompt="נא הכנס תעודת זהות של המאמן" sqref="A1:A1048576" xr:uid="{9CCA8993-050A-44DA-819E-BCC51F8A9376}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="שם פרטי" prompt="נא הכנס את שם המאמן_x000a_" sqref="B1:B1048576" xr:uid="{6D185BE6-1C70-4FBA-AF1C-284497823564}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="שם משפחה " prompt="נא הכנס את שם המשפחה של המאמן_x000a_" sqref="C1:C1048576" xr:uid="{38EA15E7-1327-4FF5-BA37-4F435035EBA9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="טלפון" prompt="נא הכנס טלפון_x000a_למשל : XXXXXXXXXX" sqref="D1:D1048576" xr:uid="{65CA328C-7349-47F3-8116-42C35E0C330C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="כתובת" prompt="נא הכנס את כתובת המגורים של המאמן" sqref="E1:E1048576" xr:uid="{36264D47-2546-4F92-8230-9FFD07BD48E5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="אימייל" prompt="נא הכנס אימייל _x000a_למשל : example@example.com" sqref="G1:G1048576" xr:uid="{9BFDFF0C-9031-4634-B4D7-1E1E4FACCB54}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="שם הקבוצה " prompt="נא הכנס את שם הקבוצה " sqref="I1:I1048576" xr:uid="{6D927ED4-D5B0-4C52-A765-95A699D4D832}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="מועדון" prompt="נא הכנס מספר מועדון _x000a_לרשותך נמצאים מספרי המועדון בצד שמאל של הדף " sqref="H1:H1048576" xr:uid="{045EAE38-18FE-4C21-9FCA-328FBDC09C78}">
+      <formula1>$K$3:$K$10</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="F1:F1048576" xr:uid="{A983D1A3-FE83-4624-8258-6A8B9098F02C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>